<commit_message>
Committing build output (including zip).  Useful if not able to build locally.
</commit_message>
<xml_diff>
--- a/docs/organization-laboratory-uv-ips.xlsx
+++ b/docs/organization-laboratory-uv-ips.xlsx
@@ -1260,8 +1260,8 @@
   </si>
   <si>
     <t>&lt;valuePeriod xmlns="http://hl7.org/fhir"&gt;
-  &lt;start value="2010-03-23T00:00:00-06:00"/&gt;
-  &lt;end value="2010-07-01T00:00:00-06:00"/&gt;
+  &lt;start value="2010-03-23T00:00:00-05:00"/&gt;
+  &lt;end value="2010-07-01T00:00:00-05:00"/&gt;
 &lt;/valuePeriod&gt;</t>
   </si>
   <si>

</xml_diff>